<commit_message>
add link to CBIP documentation / description of compound collections
</commit_message>
<xml_diff>
--- a/annotations/Pert Collection.xlsx
+++ b/annotations/Pert Collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4155" windowHeight="1005" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4155" windowHeight="1005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9941" uniqueCount="3337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9943" uniqueCount="3339">
   <si>
     <t>pert_collection</t>
   </si>
@@ -10031,6 +10031,12 @@
   </si>
   <si>
     <t>orig_row</t>
+  </si>
+  <si>
+    <t>these definitions from:</t>
+  </si>
+  <si>
+    <t>https://confluence.broadinstitute.org/display/cbip/Compound+Collections+in+the+HTS+Set</t>
   </si>
 </sst>
 </file>
@@ -10049,6 +10055,7 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -10448,10 +10455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10634,6 +10641,16 @@
       </c>
       <c r="D19" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>3337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>3338</v>
       </c>
     </row>
   </sheetData>
@@ -10654,7 +10671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2581" workbookViewId="0">
+    <sheetView topLeftCell="A2551" workbookViewId="0">
       <selection activeCell="F2585" sqref="F2585"/>
     </sheetView>
   </sheetViews>

</xml_diff>